<commit_message>
10 part of method is ended
</commit_message>
<xml_diff>
--- a/FabLab_oil_and_gas/Equations_of_state/task/коэф парного взаимодействия.xlsx
+++ b/FabLab_oil_and_gas/Equations_of_state/task/коэф парного взаимодействия.xlsx
@@ -1,17 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Ucheba\Poly_3_kurs\3_Kurs_MexMatMod\FabLab_oil_and_gas\Equations_of_state\task\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426D9D4A-85BB-4396-8FA3-E103C006AFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="348" yWindow="2796" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Лист1" sheetId="1" r:id="rId4"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
   <si>
     <t>c(ij)</t>
   </si>
@@ -89,48 +109,58 @@
   </si>
   <si>
     <t>0.135</t>
+  </si>
+  <si>
+    <t>CH41</t>
+  </si>
+  <si>
+    <t>C2H61</t>
+  </si>
+  <si>
+    <t>C3H81</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="7">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="&quot;Times New Roman&quot;"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="&quot;Times New Roman&quot;"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Times"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -140,11 +170,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -158,71 +194,55 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -412,20 +432,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,15 +488,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B2" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C2" s="7">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D2" s="7">
         <v>0.01</v>
@@ -486,13 +511,13 @@
         <v>0.03</v>
       </c>
       <c r="H2" s="7">
-        <v>0.035</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J2" s="8">
-        <v>0.025</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>13</v>
@@ -501,18 +526,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B3" s="7">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C3" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D3" s="7">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E3" s="7">
         <v>0.01</v>
@@ -539,30 +564,30 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B4" s="7">
         <v>0.01</v>
       </c>
       <c r="C4" s="7">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D4" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E4" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F4" s="7">
         <v>0.02</v>
       </c>
       <c r="G4" s="7">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H4" s="7">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>18</v>
@@ -577,7 +602,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -588,25 +613,25 @@
         <v>0.01</v>
       </c>
       <c r="D5" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E5" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F5" s="7">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="G5" s="7">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H5" s="7">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>18</v>
       </c>
       <c r="J5" s="8">
-        <v>0.095</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="K5" s="9" t="s">
         <v>21</v>
@@ -615,7 +640,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -629,19 +654,19 @@
         <v>0.02</v>
       </c>
       <c r="E6" s="7">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F6" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G6" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H6" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I6" s="10">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J6" s="8">
         <v>0.1</v>
@@ -653,7 +678,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -664,22 +689,22 @@
         <v>0.02</v>
       </c>
       <c r="D7" s="7">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E7" s="7">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F7" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G7" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H7" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I7" s="10">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J7" s="8">
         <v>0.11</v>
@@ -691,33 +716,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="7">
-        <v>0.035</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="C8" s="7">
         <v>0.02</v>
       </c>
       <c r="D8" s="7">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E8" s="7">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F8" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G8" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H8" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I8" s="10">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J8" s="8">
         <v>0.115</v>
@@ -729,7 +754,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -746,16 +771,16 @@
         <v>18</v>
       </c>
       <c r="F9" s="10">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G9" s="10">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H9" s="10">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I9" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>19</v>
@@ -767,12 +792,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="8">
-        <v>0.025</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="C10" s="8">
         <v>0.01</v>
@@ -781,7 +806,7 @@
         <v>0.09</v>
       </c>
       <c r="E10" s="8">
-        <v>0.095</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="F10" s="8">
         <v>0.1</v>
@@ -796,16 +821,16 @@
         <v>19</v>
       </c>
       <c r="J10" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K10" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L10" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -834,16 +859,16 @@
         <v>21</v>
       </c>
       <c r="J11" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K11" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L11" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>11</v>
       </c>
@@ -878,10 +903,10 @@
         <v>25</v>
       </c>
       <c r="L12" s="14">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>